<commit_message>
Added PSA talk recording.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (SPS)/Teaching/DATA606 2023 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F714E3C4-8EC3-A847-8F88-0DD4B2CDFB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1436A921-C35A-5A40-8763-A4DD2122E5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12420" yWindow="7220" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
+    <workbookView xWindow="1440" yWindow="2140" windowWidth="28800" windowHeight="17500" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
   <sheets>
     <sheet name="Meetups" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="87">
   <si>
     <t>Date</t>
   </si>
@@ -328,6 +328,20 @@
   </si>
   <si>
     <t>uTMAlvDlWAo</t>
+  </si>
+  <si>
+    <t>6:30 pm</t>
+  </si>
+  <si>
+    <t>Estimating Causality from Observational Data</t>
+  </si>
+  <si>
+    <t>Rq_od5KwqEA</t>
+  </si>
+  <si>
+    <t>Slides: https://github.com/jbryer/psa/raw/master/Slides/Intro_PSA.pdf &lt;br/&gt;
+Bookdown site: https://psa.bryer.org &lt;br/&gt;
+Github repo: https://github.com/jbryer/psa</t>
   </si>
 </sst>
 </file>
@@ -725,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12B6D5-EAC3-1C40-AC8A-3C6A227098E4}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,27 +1068,32 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>45042</v>
+        <v>45040</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="F15" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>45049</v>
+        <v>45042</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1083,7 +1102,7 @@
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -1092,7 +1111,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>45056</v>
+        <v>45049</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>11</v>
@@ -1101,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1110,7 +1129,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>45063</v>
+        <v>45056</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
@@ -1119,12 +1138,30 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45063</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
         <v>41</v>
       </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="7"/>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>